<commit_message>
add mythril bytecode results
</commit_message>
<xml_diff>
--- a/tool_results/results_analysed_numbers.xlsx
+++ b/tool_results/results_analysed_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNI\Diplom\Minimal Contracts\Templating\tool_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50654D7A-4A7F-4DBC-955F-F61EEC62AB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441DA67F-8D74-46D1-9926-F0412767123F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3612" yWindow="-17280" windowWidth="15360" windowHeight="16680" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="100">
   <si>
     <t>mythril</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>209, 210, 211, 212, 243, 244, 245, 246</t>
+  </si>
+  <si>
+    <t>Unsafe Delegatecall</t>
   </si>
 </sst>
 </file>
@@ -844,9 +847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816DF791-3565-4C2A-B7A1-D8086056D11D}">
   <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L289" sqref="L289"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2148,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C49" s="16" t="s">
         <v>22</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C50" s="16" t="s">
         <v>29</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C51" s="16" t="s">
         <v>24</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C52" s="13" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C53" s="14" t="s">
         <v>10</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C54" s="14" t="s">
         <v>11</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C55" s="14" t="s">
         <v>28</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C56" s="14" t="s">
         <v>13</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C57" s="15" t="s">
         <v>20</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C58" s="16" t="s">
         <v>21</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C59" s="16" t="s">
         <v>22</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C60" s="16" t="s">
         <v>29</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C61" s="16" t="s">
         <v>24</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>37</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C63" s="18" t="s">
         <v>10</v>
       </c>
@@ -2499,8 +2502,11 @@
         <v>38</v>
       </c>
       <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C64" s="18" t="s">
         <v>11</v>
       </c>
@@ -2526,8 +2532,11 @@
         <v>39</v>
       </c>
       <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="L64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C65" s="18" t="s">
         <v>28</v>
       </c>
@@ -2553,8 +2562,11 @@
         <v>40</v>
       </c>
       <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="L65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C66" s="18" t="s">
         <v>13</v>
       </c>
@@ -2580,8 +2592,11 @@
         <v>121</v>
       </c>
       <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="L66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C67" s="19" t="s">
         <v>20</v>
       </c>
@@ -2604,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C68" s="20" t="s">
         <v>21</v>
       </c>
@@ -2627,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C69" s="20" t="s">
         <v>22</v>
       </c>
@@ -2650,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C70" s="20" t="s">
         <v>29</v>
       </c>
@@ -2673,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C71" s="20" t="s">
         <v>24</v>
       </c>
@@ -2696,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C72" s="17" t="s">
         <v>9</v>
       </c>
@@ -2719,7 +2734,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C73" s="18" t="s">
         <v>10</v>
       </c>
@@ -2742,7 +2757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C74" s="18" t="s">
         <v>11</v>
       </c>
@@ -2765,7 +2780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C75" s="18" t="s">
         <v>28</v>
       </c>
@@ -2788,7 +2803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C76" s="18" t="s">
         <v>13</v>
       </c>
@@ -2811,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C77" s="19" t="s">
         <v>20</v>
       </c>
@@ -2834,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C78" s="20" t="s">
         <v>21</v>
       </c>
@@ -2857,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C79" s="20" t="s">
         <v>22</v>
       </c>
@@ -2880,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C80" s="20" t="s">
         <v>29</v>
       </c>
@@ -5994,10 +6009,18 @@
       <c r="E204" s="25">
         <v>35</v>
       </c>
-      <c r="F204" s="5"/>
-      <c r="G204" s="5"/>
-      <c r="H204" s="5"/>
-      <c r="I204" s="5"/>
+      <c r="F204" s="5">
+        <v>0</v>
+      </c>
+      <c r="G204" s="5">
+        <v>3</v>
+      </c>
+      <c r="H204" s="5">
+        <v>0</v>
+      </c>
+      <c r="I204" s="5">
+        <v>32</v>
+      </c>
       <c r="J204" s="2"/>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.35">
@@ -6039,10 +6062,18 @@
       <c r="E206" s="26">
         <v>10</v>
       </c>
-      <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
-      <c r="I206" s="3"/>
+      <c r="F206" s="3">
+        <v>0</v>
+      </c>
+      <c r="G206" s="3">
+        <v>0</v>
+      </c>
+      <c r="H206" s="3">
+        <v>0</v>
+      </c>
+      <c r="I206" s="3">
+        <v>10</v>
+      </c>
       <c r="J206" s="2"/>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.35">
@@ -6098,7 +6129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="209" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C209" s="7" t="s">
         <v>20</v>
       </c>
@@ -6109,13 +6140,21 @@
         <f>3*8+4</f>
         <v>28</v>
       </c>
-      <c r="F209" s="7"/>
-      <c r="G209" s="7"/>
-      <c r="H209" s="7"/>
-      <c r="I209" s="7"/>
+      <c r="F209" s="7">
+        <v>12</v>
+      </c>
+      <c r="G209" s="7">
+        <v>0</v>
+      </c>
+      <c r="H209" s="7">
+        <v>16</v>
+      </c>
+      <c r="I209" s="7">
+        <v>0</v>
+      </c>
       <c r="J209" s="2"/>
     </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C210" s="4" t="s">
         <v>21</v>
       </c>
@@ -6139,7 +6178,7 @@
       </c>
       <c r="J210" s="2"/>
     </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C211" s="4" t="s">
         <v>22</v>
       </c>
@@ -6149,13 +6188,24 @@
       <c r="E211" s="28">
         <v>8</v>
       </c>
-      <c r="F211" s="4"/>
-      <c r="G211" s="4"/>
-      <c r="H211" s="4"/>
-      <c r="I211" s="4"/>
+      <c r="F211" s="4">
+        <v>0</v>
+      </c>
+      <c r="G211" s="4">
+        <v>0</v>
+      </c>
+      <c r="H211" s="4">
+        <v>8</v>
+      </c>
+      <c r="I211" s="4">
+        <v>0</v>
+      </c>
       <c r="J211" s="2"/>
-    </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="M211" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="212" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C212" s="4" t="s">
         <v>23</v>
       </c>
@@ -6179,7 +6229,7 @@
       </c>
       <c r="J212" s="2"/>
     </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C213" s="4" t="s">
         <v>24</v>
       </c>
@@ -6203,7 +6253,7 @@
       </c>
       <c r="J213" s="2"/>
     </row>
-    <row r="214" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C214" s="5" t="s">
         <v>9</v>
       </c>
@@ -6227,7 +6277,7 @@
       </c>
       <c r="J214" s="2"/>
     </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C215" s="3" t="s">
         <v>10</v>
       </c>
@@ -6251,7 +6301,7 @@
       </c>
       <c r="J215" s="2"/>
     </row>
-    <row r="216" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C216" s="3" t="s">
         <v>11</v>
       </c>
@@ -6275,7 +6325,7 @@
       </c>
       <c r="J216" s="2"/>
     </row>
-    <row r="217" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C217" s="3" t="s">
         <v>12</v>
       </c>
@@ -6299,7 +6349,7 @@
       </c>
       <c r="J217" s="2"/>
     </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C218" s="3" t="s">
         <v>13</v>
       </c>
@@ -6323,7 +6373,7 @@
       </c>
       <c r="J218" s="2"/>
     </row>
-    <row r="219" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C219" s="7" t="s">
         <v>20</v>
       </c>
@@ -6347,7 +6397,7 @@
       </c>
       <c r="J219" s="2"/>
     </row>
-    <row r="220" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C220" s="4" t="s">
         <v>21</v>
       </c>
@@ -6371,7 +6421,7 @@
       </c>
       <c r="J220" s="2"/>
     </row>
-    <row r="221" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C221" s="4" t="s">
         <v>22</v>
       </c>
@@ -6395,7 +6445,7 @@
       </c>
       <c r="J221" s="2"/>
     </row>
-    <row r="222" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C222" s="4" t="s">
         <v>23</v>
       </c>
@@ -6419,7 +6469,7 @@
       </c>
       <c r="J222" s="2"/>
     </row>
-    <row r="223" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C223" s="4" t="s">
         <v>24</v>
       </c>
@@ -6443,7 +6493,7 @@
       </c>
       <c r="J223" s="2"/>
     </row>
-    <row r="224" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B224" t="s">
         <v>19</v>
       </c>
@@ -6456,10 +6506,18 @@
       <c r="E224" s="29">
         <v>35</v>
       </c>
-      <c r="F224" s="9"/>
-      <c r="G224" s="9"/>
-      <c r="H224" s="9"/>
-      <c r="I224" s="9"/>
+      <c r="F224" s="9">
+        <v>0</v>
+      </c>
+      <c r="G224" s="9">
+        <v>3</v>
+      </c>
+      <c r="H224" s="9">
+        <v>0</v>
+      </c>
+      <c r="I224" s="9">
+        <v>32</v>
+      </c>
       <c r="J224" s="2"/>
     </row>
     <row r="225" spans="3:12" x14ac:dyDescent="0.35">
@@ -6501,10 +6559,18 @@
       <c r="E226" s="30">
         <v>10</v>
       </c>
-      <c r="F226" s="10"/>
-      <c r="G226" s="10"/>
-      <c r="H226" s="10"/>
-      <c r="I226" s="10"/>
+      <c r="F226" s="10">
+        <v>0</v>
+      </c>
+      <c r="G226" s="10">
+        <v>0</v>
+      </c>
+      <c r="H226" s="10">
+        <v>0</v>
+      </c>
+      <c r="I226" s="10">
+        <v>10</v>
+      </c>
       <c r="J226" s="2"/>
     </row>
     <row r="227" spans="3:12" x14ac:dyDescent="0.35">
@@ -6570,10 +6636,18 @@
       <c r="E229" s="31">
         <v>28</v>
       </c>
-      <c r="F229" s="11"/>
-      <c r="G229" s="11"/>
-      <c r="H229" s="11"/>
-      <c r="I229" s="11"/>
+      <c r="F229" s="11">
+        <v>12</v>
+      </c>
+      <c r="G229" s="11">
+        <v>0</v>
+      </c>
+      <c r="H229" s="11">
+        <v>16</v>
+      </c>
+      <c r="I229" s="11">
+        <v>0</v>
+      </c>
       <c r="J229" s="2"/>
     </row>
     <row r="230" spans="3:12" x14ac:dyDescent="0.35">
@@ -6610,10 +6684,18 @@
       <c r="E231" s="32">
         <v>8</v>
       </c>
-      <c r="F231" s="12"/>
-      <c r="G231" s="12"/>
-      <c r="H231" s="12"/>
-      <c r="I231" s="12"/>
+      <c r="F231" s="12">
+        <v>0</v>
+      </c>
+      <c r="G231" s="12">
+        <v>0</v>
+      </c>
+      <c r="H231" s="12">
+        <v>8</v>
+      </c>
+      <c r="I231" s="12">
+        <v>0</v>
+      </c>
       <c r="J231" s="2"/>
     </row>
     <row r="232" spans="3:12" x14ac:dyDescent="0.35">
@@ -6919,10 +7001,18 @@
       <c r="E244" s="33">
         <v>35</v>
       </c>
-      <c r="F244" s="13"/>
-      <c r="G244" s="13"/>
-      <c r="H244" s="13"/>
-      <c r="I244" s="13"/>
+      <c r="F244" s="13">
+        <v>0</v>
+      </c>
+      <c r="G244" s="13">
+        <v>3</v>
+      </c>
+      <c r="H244" s="13">
+        <v>0</v>
+      </c>
+      <c r="I244" s="13">
+        <v>32</v>
+      </c>
       <c r="J244" s="2"/>
     </row>
     <row r="245" spans="2:12" x14ac:dyDescent="0.35">
@@ -6964,10 +7054,18 @@
       <c r="E246" s="34">
         <v>10</v>
       </c>
-      <c r="F246" s="14"/>
-      <c r="G246" s="14"/>
-      <c r="H246" s="14"/>
-      <c r="I246" s="14"/>
+      <c r="F246" s="14">
+        <v>0</v>
+      </c>
+      <c r="G246" s="14">
+        <v>0</v>
+      </c>
+      <c r="H246" s="14">
+        <v>0</v>
+      </c>
+      <c r="I246" s="14">
+        <v>10</v>
+      </c>
       <c r="J246" s="2"/>
     </row>
     <row r="247" spans="2:12" x14ac:dyDescent="0.35">
@@ -7033,10 +7131,18 @@
       <c r="E249" s="35">
         <v>28</v>
       </c>
-      <c r="F249" s="15"/>
-      <c r="G249" s="15"/>
-      <c r="H249" s="15"/>
-      <c r="I249" s="15"/>
+      <c r="F249" s="15">
+        <v>12</v>
+      </c>
+      <c r="G249" s="15">
+        <v>0</v>
+      </c>
+      <c r="H249" s="15">
+        <v>16</v>
+      </c>
+      <c r="I249" s="15">
+        <v>0</v>
+      </c>
       <c r="J249" s="2"/>
     </row>
     <row r="250" spans="2:12" x14ac:dyDescent="0.35">
@@ -7073,10 +7179,18 @@
       <c r="E251" s="36">
         <v>8</v>
       </c>
-      <c r="F251" s="16"/>
-      <c r="G251" s="16"/>
-      <c r="H251" s="16"/>
-      <c r="I251" s="16"/>
+      <c r="F251" s="16">
+        <v>0</v>
+      </c>
+      <c r="G251" s="16">
+        <v>0</v>
+      </c>
+      <c r="H251" s="16">
+        <v>8</v>
+      </c>
+      <c r="I251" s="16">
+        <v>0</v>
+      </c>
       <c r="J251" s="2"/>
     </row>
     <row r="252" spans="2:12" x14ac:dyDescent="0.35">
@@ -7380,10 +7494,18 @@
       <c r="E264" s="37">
         <v>35</v>
       </c>
-      <c r="F264" s="17"/>
-      <c r="G264" s="17"/>
-      <c r="H264" s="17"/>
-      <c r="I264" s="17"/>
+      <c r="F264" s="17">
+        <v>0</v>
+      </c>
+      <c r="G264" s="17">
+        <v>3</v>
+      </c>
+      <c r="H264" s="17">
+        <v>0</v>
+      </c>
+      <c r="I264" s="17">
+        <v>32</v>
+      </c>
       <c r="J264" s="2"/>
     </row>
     <row r="265" spans="2:12" x14ac:dyDescent="0.35">
@@ -7425,10 +7547,18 @@
       <c r="E266" s="38">
         <v>10</v>
       </c>
-      <c r="F266" s="18"/>
-      <c r="G266" s="18"/>
-      <c r="H266" s="18"/>
-      <c r="I266" s="18"/>
+      <c r="F266" s="18">
+        <v>0</v>
+      </c>
+      <c r="G266" s="18">
+        <v>0</v>
+      </c>
+      <c r="H266" s="18">
+        <v>0</v>
+      </c>
+      <c r="I266" s="18">
+        <v>10</v>
+      </c>
       <c r="J266" s="2"/>
     </row>
     <row r="267" spans="2:12" x14ac:dyDescent="0.35">
@@ -7494,10 +7624,18 @@
       <c r="E269" s="39">
         <v>28</v>
       </c>
-      <c r="F269" s="19"/>
-      <c r="G269" s="19"/>
-      <c r="H269" s="19"/>
-      <c r="I269" s="19"/>
+      <c r="F269" s="19">
+        <v>12</v>
+      </c>
+      <c r="G269" s="19">
+        <v>0</v>
+      </c>
+      <c r="H269" s="19">
+        <v>16</v>
+      </c>
+      <c r="I269" s="19">
+        <v>0</v>
+      </c>
       <c r="J269" s="2"/>
     </row>
     <row r="270" spans="2:12" x14ac:dyDescent="0.35">
@@ -7534,10 +7672,18 @@
       <c r="E271" s="40">
         <v>8</v>
       </c>
-      <c r="F271" s="20"/>
-      <c r="G271" s="20"/>
-      <c r="H271" s="20"/>
-      <c r="I271" s="20"/>
+      <c r="F271" s="20">
+        <v>0</v>
+      </c>
+      <c r="G271" s="20">
+        <v>0</v>
+      </c>
+      <c r="H271" s="20">
+        <v>8</v>
+      </c>
+      <c r="I271" s="20">
+        <v>0</v>
+      </c>
       <c r="J271" s="2"/>
     </row>
     <row r="272" spans="2:12" x14ac:dyDescent="0.35">
@@ -7841,10 +7987,18 @@
       <c r="E284" s="41">
         <v>35</v>
       </c>
-      <c r="F284" s="21"/>
-      <c r="G284" s="21"/>
-      <c r="H284" s="21"/>
-      <c r="I284" s="21"/>
+      <c r="F284" s="21">
+        <v>0</v>
+      </c>
+      <c r="G284" s="21">
+        <v>3</v>
+      </c>
+      <c r="H284" s="21">
+        <v>0</v>
+      </c>
+      <c r="I284" s="21">
+        <v>32</v>
+      </c>
       <c r="J284" s="2"/>
     </row>
     <row r="285" spans="2:12" x14ac:dyDescent="0.35">
@@ -7886,10 +8040,18 @@
       <c r="E286" s="42">
         <v>10</v>
       </c>
-      <c r="F286" s="22"/>
-      <c r="G286" s="22"/>
-      <c r="H286" s="22"/>
-      <c r="I286" s="22"/>
+      <c r="F286" s="22">
+        <v>0</v>
+      </c>
+      <c r="G286" s="22">
+        <v>0</v>
+      </c>
+      <c r="H286" s="22">
+        <v>0</v>
+      </c>
+      <c r="I286" s="22">
+        <v>10</v>
+      </c>
       <c r="J286" s="2"/>
     </row>
     <row r="287" spans="2:12" x14ac:dyDescent="0.35">
@@ -7955,10 +8117,18 @@
       <c r="E289" s="43">
         <v>28</v>
       </c>
-      <c r="F289" s="23"/>
-      <c r="G289" s="23"/>
-      <c r="H289" s="23"/>
-      <c r="I289" s="23"/>
+      <c r="F289" s="23">
+        <v>12</v>
+      </c>
+      <c r="G289" s="23">
+        <v>0</v>
+      </c>
+      <c r="H289" s="23">
+        <v>16</v>
+      </c>
+      <c r="I289" s="23">
+        <v>0</v>
+      </c>
       <c r="J289" s="2"/>
     </row>
     <row r="290" spans="3:10" x14ac:dyDescent="0.35">
@@ -7995,10 +8165,18 @@
       <c r="E291" s="44">
         <v>8</v>
       </c>
-      <c r="F291" s="24"/>
-      <c r="G291" s="24"/>
-      <c r="H291" s="24"/>
-      <c r="I291" s="24"/>
+      <c r="F291" s="24">
+        <v>0</v>
+      </c>
+      <c r="G291" s="24">
+        <v>0</v>
+      </c>
+      <c r="H291" s="24">
+        <v>8</v>
+      </c>
+      <c r="I291" s="24">
+        <v>0</v>
+      </c>
       <c r="J291" s="2"/>
     </row>
     <row r="292" spans="3:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added 2 additional tests
</commit_message>
<xml_diff>
--- a/tool_results/results_analysed_numbers.xlsx
+++ b/tool_results/results_analysed_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNI\Diplom\Minimal Contracts\Templating\tool_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65133F6-6EA1-489F-AF6C-02886D98C401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4387AF-AC4D-4CDA-8BC4-577D336B505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3720" yWindow="-17388" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -440,13 +440,13 @@
     <t>Recall = TP / (TP + FN)</t>
   </si>
   <si>
-    <t>Specifity</t>
-  </si>
-  <si>
     <t>Specifity  = TN / (TN + FP)</t>
   </si>
   <si>
     <t>Accuracy = (TP + TN) / N</t>
+  </si>
+  <si>
+    <t>Specificity</t>
   </si>
 </sst>
 </file>
@@ -9963,8 +9963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995A027-CBA2-444C-83FA-6EB946FF890B}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9994,10 +9994,10 @@
         <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -10189,7 +10189,7 @@
         <v>0.95238095238095233</v>
       </c>
       <c r="J4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -11725,7 +11725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13FB626-F218-4B99-B9CF-F14B8A51FAA4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
separated function and constructor results
</commit_message>
<xml_diff>
--- a/tool_results/results_analysed_numbers.xlsx
+++ b/tool_results/results_analysed_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNI\Diplom\Minimal Contracts\Templating\tool_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77231A10-BA6E-4B9D-AF46-C2F87620F5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA39C3-00D9-47D6-A4DA-1A48D29DBA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="1" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{7EB0B72A-79A8-4C26-A6CB-77D713D26FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="145">
   <si>
     <t>mythril</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Overall results for each tool</t>
   </si>
   <si>
-    <t>Mythril</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -384,16 +381,7 @@
     <t>Recall</t>
   </si>
   <si>
-    <t>Slither</t>
-  </si>
-  <si>
-    <t>Confuzzius</t>
-  </si>
-  <si>
     <t>Results by low-level construct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mythril </t>
   </si>
   <si>
     <t>Category</t>
@@ -464,11 +452,59 @@
   <si>
     <t>Contract_address_uc_data2_8; Contract_address_uc_data_8; Contract_uc_data_8</t>
   </si>
+  <si>
+    <t>F1-Score</t>
+  </si>
+  <si>
+    <t>n function</t>
+  </si>
+  <si>
+    <t>Mythril c+f</t>
+  </si>
+  <si>
+    <t>Slither c+f</t>
+  </si>
+  <si>
+    <t>Confuzzius c+f</t>
+  </si>
+  <si>
+    <t>Mythril f</t>
+  </si>
+  <si>
+    <t>Mythril c</t>
+  </si>
+  <si>
+    <t>n constructor</t>
+  </si>
+  <si>
+    <t>Slither f</t>
+  </si>
+  <si>
+    <t>Slither c</t>
+  </si>
+  <si>
+    <t>Confuzzius f</t>
+  </si>
+  <si>
+    <t>TP = f</t>
+  </si>
+  <si>
+    <t>FP = g</t>
+  </si>
+  <si>
+    <t>TN = i</t>
+  </si>
+  <si>
+    <t>FN = h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +596,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -582,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -635,6 +677,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -748,7 +792,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -762,12 +806,12 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-4507-4480-B46F-15163A9F01A4}"/>
+                <c16:uniqueId val="{00000001-AA98-482E-BBD9-23E9C79A3208}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="2"/>
+            <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -781,7 +825,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-4507-4480-B46F-15163A9F01A4}"/>
+                <c16:uniqueId val="{00000003-AA98-482E-BBD9-23E9C79A3208}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -801,17 +845,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$2:$D$4</c:f>
+              <c:f>metrics!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.87058823529411766</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.83174603174603179</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.76470588235294112</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.60504201680672265</c:v>
                 </c:pt>
               </c:numCache>
@@ -953,6 +1009,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -960,7 +1017,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1089,7 +1145,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$22:$D$26</c:f>
+              <c:f>metrics!$D$54:$D$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1146,7 +1202,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$27:$D$31</c:f>
+              <c:f>metrics!$D$70:$D$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1203,7 +1259,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$32:$D$36</c:f>
+              <c:f>metrics!$D$86:$D$90</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1525,7 +1581,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$6:$D$10</c:f>
+              <c:f>metrics!$D$11:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1683,6 +1739,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1690,7 +1747,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1844,7 +1900,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$6:$D$10</c:f>
+              <c:f>metrics!$D$11:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1890,7 +1946,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$11:$D$15</c:f>
+              <c:f>metrics!$D$27:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1936,7 +1992,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>metrics!$D$16:$D$20</c:f>
+              <c:f>metrics!$D$43:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2094,6 +2150,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2101,7 +2158,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4233,8 +4289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816DF791-3565-4C2A-B7A1-D8086056D11D}">
   <dimension ref="A1:N303"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
@@ -4353,7 +4409,7 @@
         <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -11865,7 +11921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818B4C76-8770-46BA-BF7E-6B24BFF81621}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
@@ -12283,7 +12339,7 @@
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -12310,7 +12366,7 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.35">
@@ -12337,7 +12393,7 @@
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.35">
@@ -12434,10 +12490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995A027-CBA2-444C-83FA-6EB946FF890B}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12447,59 +12503,69 @@
     <col min="10" max="10" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" t="s">
         <v>118</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>119</v>
       </c>
-      <c r="O1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="D2" cm="1">
         <f t="array" ref="D2">_xlfn.LET(
@@ -12542,45 +12608,149 @@
 )</f>
         <v>0.90793650793650793</v>
       </c>
+      <c r="H2">
+        <f>(2*E2*F2)/(E2+F2)</f>
+        <v>0.85767097966728278</v>
+      </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L2">
         <v>595</v>
       </c>
       <c r="M2">
+        <v>315</v>
+      </c>
+      <c r="N2">
+        <f>L2-M2</f>
+        <v>280</v>
+      </c>
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>101</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>103</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>202</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>204</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" cm="1">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B3" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47" cm="1">
         <f t="array" ref="D3">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,7,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,7,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/M2
+)</f>
+        <v>0.83174603174603179</v>
+      </c>
+      <c r="E3" s="47" cm="1">
+        <f t="array" ref="E3">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="47" cm="1">
+        <f t="array" ref="F3">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.82857142857142863</v>
+      </c>
+      <c r="G3" s="47" cm="1">
+        <f t="array" ref="G3">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,2,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,7,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8342857142857143</v>
+      </c>
+      <c r="H3" s="47">
+        <f t="shared" ref="H3:H4" si="0">(2*E3*F3)/(E3+F3)</f>
+        <v>0.81403508771929833</v>
+      </c>
+      <c r="J3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" cm="1">
+        <f t="array" ref="D4">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,17,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,17,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/N2
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="E4" s="10" cm="1">
+        <f t="array" ref="E4">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" cm="1">
+        <f t="array" ref="F4">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.82857142857142863</v>
+      </c>
+      <c r="G4" s="10" cm="1">
+        <f t="array" ref="G4">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,12,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,17,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>0.90625</v>
+      </c>
+      <c r="J4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" cm="1">
+        <f t="array" ref="D5">_xlfn.LET(
   _xlpm.fRange, _xlfn._xlws.FILTER(results!F103:'results'!F202, MOD(ROW(results!F103:'results'!F202)-103,5)=0),
   _xlpm.iRange, _xlfn._xlws.FILTER(results!I103:'results'!I202, MOD(ROW(results!I103:'results'!I202)-103,5)=0),
   SUM(_xlpm.fRange + _xlpm.iRange)/L2
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E3" cm="1">
-        <f t="array" ref="E3">_xlfn.LET(
+      <c r="E5" cm="1">
+        <f t="array" ref="E5">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,103,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12590,8 +12760,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F3" cm="1">
-        <f t="array" ref="F3">_xlfn.LET(
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,103,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12601,8 +12771,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G3" cm="1">
-        <f t="array" ref="G3">_xlfn.LET(
+      <c r="G5" cm="1">
+        <f t="array" ref="G5">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,103,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12612,24 +12782,118 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="J3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" cm="1">
-        <f t="array" ref="D4">_xlfn.LET(
+      <c r="H5">
+        <f>(2*E5*F5)/(E5+F5)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B6" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47" cm="1">
+        <f t="array" ref="D6">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,108,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,108,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/M2
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E6" s="47" cm="1">
+        <f t="array" ref="E6">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="47" cm="1">
+        <f t="array" ref="F6">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="47" cm="1">
+        <f t="array" ref="G6">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,103,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,108,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="47">
+        <f t="shared" ref="H6:H7" si="1">(2*E6*F6)/(E6+F6)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" cm="1">
+        <f t="array" ref="D7">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,118,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,118,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/N2
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="10" cm="1">
+        <f t="array" ref="E7">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" cm="1">
+        <f t="array" ref="F7">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="10" cm="1">
+        <f t="array" ref="G7">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,113,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,118,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" cm="1">
+        <f t="array" ref="D8">_xlfn.LET(
   _xlpm.fRange, _xlfn._xlws.FILTER(results!F204:'results'!F304, MOD(ROW(results!F204:'results'!F304)-204,5)=0),
   _xlpm.iRange, _xlfn._xlws.FILTER(results!I204:'results'!I304, MOD(ROW(results!I204:'results'!I304)-204,5)=0),
   SUM(_xlpm.fRange + _xlpm.iRange)/L2
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E4" cm="1">
-        <f t="array" ref="E4">_xlfn.LET(
+      <c r="E8" cm="1">
+        <f t="array" ref="E8">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,204,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12639,8 +12903,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F4" cm="1">
-        <f t="array" ref="F4">_xlfn.LET(
+      <c r="F8" cm="1">
+        <f t="array" ref="F8">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,204,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12650,8 +12914,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G4" cm="1">
-        <f t="array" ref="G4">_xlfn.LET(
+      <c r="G8" cm="1">
+        <f t="array" ref="G8">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,204,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12661,33 +12925,76 @@
 )</f>
         <v>0.95238095238095233</v>
       </c>
-      <c r="J4" t="s">
+      <c r="H8">
+        <f>(2*E8*F8)/(E8+F8)</f>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B9" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47" cm="1">
+        <f t="array" ref="D9">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,209,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,209,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/M2
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E9" s="47" cm="1">
+        <f t="array" ref="E9">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="47" cm="1">
+        <f t="array" ref="F9">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G9" s="47" cm="1">
+        <f t="array" ref="G9">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,204,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,209,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H9" s="47">
+        <f>(2*E9*F9)/(E9+F9)</f>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="M5" t="s">
-        <v>130</v>
-      </c>
-      <c r="O5" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R10" t="s">
+        <v>127</v>
+      </c>
+      <c r="T10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" cm="1">
-        <f t="array" ref="D6">_xlfn.LET(
+      <c r="C11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="3" cm="1">
+        <f t="array" ref="D11">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,6,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12698,8 +13005,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E6" cm="1">
-        <f t="array" ref="E6">_xlfn.LET(
+      <c r="E11" s="3" cm="1">
+        <f t="array" ref="E11">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,6,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12709,8 +13016,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F6" cm="1">
-        <f t="array" ref="F6">_xlfn.LET(
+      <c r="F11" s="3" cm="1">
+        <f t="array" ref="F11">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,6,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12720,8 +13027,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G6" cm="1">
-        <f t="array" ref="G6">_xlfn.LET(
+      <c r="G11" s="3" cm="1">
+        <f t="array" ref="G11">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,6,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12731,25 +13038,30 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="M6">
+      <c r="H11" s="3">
+        <f t="shared" ref="H11:H47" si="2">(2*E11*F11)/(E11+F11)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="P11">
         <f>SUM(results!F7,results!F17,results!F27,results!F37,results!F47,results!F57,results!F67,results!F77,results!F87,results!F97)</f>
         <v>232</v>
       </c>
-      <c r="O6">
+      <c r="R11">
         <f>SUM(results!F108,results!F118,results!F128,results!F138,results!F148,results!F158,results!F168,results!F178,results!F188,results!F198)</f>
         <v>140</v>
       </c>
-      <c r="Q6">
+      <c r="T11">
         <f>SUM(results!F209,results!F219,results!F229,results!F239,results!F249,results!F259,results!F269,results!F279,results!F289,results!F299)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" cm="1">
-        <f t="array" ref="D7">_xlfn.LET(
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="3" cm="1">
+        <f t="array" ref="D12">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,3,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12760,8 +13072,8 @@
 )</f>
         <v>0.85882352941176465</v>
       </c>
-      <c r="E7" cm="1">
-        <f t="array" ref="E7">_xlfn.LET(
+      <c r="E12" s="3" cm="1">
+        <f t="array" ref="E12">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,3,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12771,8 +13083,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F7" cm="1">
-        <f t="array" ref="F7">_xlfn.LET(
+      <c r="F12" s="3" cm="1">
+        <f t="array" ref="F12">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,3,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12782,8 +13094,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="G7" cm="1">
-        <f t="array" ref="G7">_xlfn.LET(
+      <c r="G12" s="3" cm="1">
+        <f t="array" ref="G12">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,3,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12793,13 +13105,18 @@
 )</f>
         <v>0.91111111111111109</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" cm="1">
-        <f t="array" ref="D8">_xlfn.LET(
+      <c r="H12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8421052631578948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="3" cm="1">
+        <f t="array" ref="D13">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,4,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12810,8 +13127,8 @@
 )</f>
         <v>0.85882352941176465</v>
       </c>
-      <c r="E8" cm="1">
-        <f t="array" ref="E8">_xlfn.LET(
+      <c r="E13" s="3" cm="1">
+        <f t="array" ref="E13">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,4,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12821,8 +13138,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F8" cm="1">
-        <f t="array" ref="F8">_xlfn.LET(
+      <c r="F13" s="3" cm="1">
+        <f t="array" ref="F13">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,4,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12832,8 +13149,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="G8" cm="1">
-        <f t="array" ref="G8">_xlfn.LET(
+      <c r="G13" s="3" cm="1">
+        <f t="array" ref="G13">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,4,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12843,13 +13160,18 @@
 )</f>
         <v>0.91111111111111109</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" cm="1">
-        <f t="array" ref="D9">_xlfn.LET(
+      <c r="H13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8421052631578948</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="3" cm="1">
+        <f t="array" ref="D14">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,25,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12860,8 +13182,8 @@
 )</f>
         <v>0.83823529411764708</v>
       </c>
-      <c r="E9" cm="1">
-        <f t="array" ref="E9">_xlfn.LET(
+      <c r="E14" s="3" cm="1">
+        <f t="array" ref="E14">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,25,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12871,8 +13193,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F9" cm="1">
-        <f t="array" ref="F9">_xlfn.LET(
+      <c r="F14" s="3" cm="1">
+        <f t="array" ref="F14">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,25,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12882,8 +13204,8 @@
 )</f>
         <v>0.75</v>
       </c>
-      <c r="G9" cm="1">
-        <f t="array" ref="G9">_xlfn.LET(
+      <c r="G14" s="3" cm="1">
+        <f t="array" ref="G14">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,25,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12893,13 +13215,19 @@
 )</f>
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" cm="1">
-        <f t="array" ref="D10">_xlfn.LET(
+      <c r="H14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.81355932203389825</v>
+      </c>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="3" cm="1">
+        <f t="array" ref="D15">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,5,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12910,8 +13238,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E10" cm="1">
-        <f t="array" ref="E10">_xlfn.LET(
+      <c r="E15" s="3" cm="1">
+        <f t="array" ref="E15">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,5,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12921,8 +13249,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F10" cm="1">
-        <f t="array" ref="F10">_xlfn.LET(
+      <c r="F15" s="3" cm="1">
+        <f t="array" ref="F15">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,5,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12932,8 +13260,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G10" cm="1">
-        <f t="array" ref="G10">_xlfn.LET(
+      <c r="G15" s="3" cm="1">
+        <f t="array" ref="G15">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,5,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12943,16 +13271,454 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="H15" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="10" cm="1">
+        <f t="array" ref="D16">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,11,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,11,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,11,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E16" s="10" cm="1">
+        <f t="array" ref="E16">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="10" cm="1">
+        <f t="array" ref="F16">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="10" cm="1">
+        <f t="array" ref="G16">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,6,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,11,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="10" cm="1">
+        <f t="array" ref="D17">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,8,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,8,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,8,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.82222222222222219</v>
+      </c>
+      <c r="E17" s="10" cm="1">
+        <f t="array" ref="E17">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="10" cm="1">
+        <f t="array" ref="F17">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="10" cm="1">
+        <f t="array" ref="G17">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,3,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,8,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.84</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.80000000000000016</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="10" cm="1">
+        <f t="array" ref="D18">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,9,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,9,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,9,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.82222222222222219</v>
+      </c>
+      <c r="E18" s="10" cm="1">
+        <f t="array" ref="E18">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="10" cm="1">
+        <f t="array" ref="F18">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G18" s="10" cm="1">
+        <f t="array" ref="G18">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,4,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,9,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.84</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.80000000000000016</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="10" cm="1">
+        <f t="array" ref="D19">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,30,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,30,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!E:E, _xlfn.SEQUENCE(4,1,30,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="E19" s="10" cm="1">
+        <f t="array" ref="E19">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="10" cm="1">
+        <f t="array" ref="F19">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!H:H, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G19" s="10" cm="1">
+        <f t="array" ref="G19">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,25,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,30,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.85</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="2"/>
+        <v>0.77419354838709686</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D11" cm="1">
-        <f t="array" ref="D11">_xlfn.LET(
+      <c r="D20" s="10" cm="1">
+        <f t="array" ref="D20">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,10,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,10,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!E:E, _xlfn.SEQUENCE(1,1,10,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E20" s="10" cm="1">
+        <f t="array" ref="E20">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="10" cm="1">
+        <f t="array" ref="F20">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!H:H, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="10" cm="1">
+        <f t="array" ref="G20">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,5,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,10,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="18" cm="1">
+        <f t="array" ref="D21">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,21,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,21,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,21,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="18" cm="1">
+        <f t="array" ref="E21">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="18" cm="1">
+        <f t="array" ref="F21">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="18" cm="1">
+        <f t="array" ref="G21">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,16,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,21,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="18" cm="1">
+        <f t="array" ref="D22">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,18,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,18,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,18,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.9</v>
+      </c>
+      <c r="E22" s="18" cm="1">
+        <f t="array" ref="E22">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="18" cm="1">
+        <f t="array" ref="F22">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G22" s="18" cm="1">
+        <f t="array" ref="G22">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,13,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,18,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="18">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="18" cm="1">
+        <f t="array" ref="D23">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,19,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,19,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,19,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.9</v>
+      </c>
+      <c r="E23" s="18" cm="1">
+        <f t="array" ref="E23">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="18" cm="1">
+        <f t="array" ref="F23">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G23" s="18" cm="1">
+        <f t="array" ref="G23">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,14,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,19,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="18">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="18" cm="1">
+        <f t="array" ref="D24">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,40,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,40,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!E:E, _xlfn.SEQUENCE(4,1,40,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.875</v>
+      </c>
+      <c r="E24" s="18" cm="1">
+        <f t="array" ref="E24">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="18" cm="1">
+        <f t="array" ref="F24">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!H:H, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G24" s="18" cm="1">
+        <f t="array" ref="G24">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,35,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,40,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="2"/>
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="18" cm="1">
+        <f t="array" ref="D25">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,20,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,20,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!E:E, _xlfn.SEQUENCE(1,1,20,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="18" cm="1">
+        <f t="array" ref="E25">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="18" cm="1">
+        <f t="array" ref="F25">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!H:H, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="18" cm="1">
+        <f t="array" ref="G25">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,15,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,20,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="3" cm="1">
+        <f t="array" ref="D27">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,107,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -12963,8 +13729,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E11" cm="1">
-        <f t="array" ref="E11">_xlfn.LET(
+      <c r="E27" s="3" cm="1">
+        <f t="array" ref="E27">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,107,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12974,8 +13740,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F11" cm="1">
-        <f t="array" ref="F11">_xlfn.LET(
+      <c r="F27" s="3" cm="1">
+        <f t="array" ref="F27">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,107,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -12985,8 +13751,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G11" cm="1">
-        <f t="array" ref="G11">_xlfn.LET(
+      <c r="G27" s="3" cm="1">
+        <f t="array" ref="G27">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,107,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -12996,13 +13762,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" cm="1">
-        <f t="array" ref="D12">_xlfn.LET(
+      <c r="H27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="3" cm="1">
+        <f t="array" ref="D28">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,104,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13013,8 +13784,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E12" cm="1">
-        <f t="array" ref="E12">_xlfn.LET(
+      <c r="E28" s="3" cm="1">
+        <f t="array" ref="E28">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,104,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13024,8 +13795,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F12" cm="1">
-        <f t="array" ref="F12">_xlfn.LET(
+      <c r="F28" s="3" cm="1">
+        <f t="array" ref="F28">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,104,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13035,8 +13806,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G12" cm="1">
-        <f t="array" ref="G12">_xlfn.LET(
+      <c r="G28" s="3" cm="1">
+        <f t="array" ref="G28">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,104,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13046,13 +13817,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" cm="1">
-        <f t="array" ref="D13">_xlfn.LET(
+      <c r="H28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="3" cm="1">
+        <f t="array" ref="D29">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,105,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13063,8 +13839,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E13" cm="1">
-        <f t="array" ref="E13">_xlfn.LET(
+      <c r="E29" s="3" cm="1">
+        <f t="array" ref="E29">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,105,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13074,8 +13850,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F13" cm="1">
-        <f t="array" ref="F13">_xlfn.LET(
+      <c r="F29" s="3" cm="1">
+        <f t="array" ref="F29">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,105,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13085,8 +13861,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G13" cm="1">
-        <f t="array" ref="G13">_xlfn.LET(
+      <c r="G29" s="3" cm="1">
+        <f t="array" ref="G29">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,105,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13096,13 +13872,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" cm="1">
-        <f t="array" ref="D14">_xlfn.LET(
+      <c r="H29" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="3" cm="1">
+        <f t="array" ref="D30">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,126,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13113,8 +13894,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E14" cm="1">
-        <f t="array" ref="E14">_xlfn.LET(
+      <c r="E30" s="3" cm="1">
+        <f t="array" ref="E30">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,126,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13124,8 +13905,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F14" cm="1">
-        <f t="array" ref="F14">_xlfn.LET(
+      <c r="F30" s="3" cm="1">
+        <f t="array" ref="F30">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,126,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13135,8 +13916,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G14" cm="1">
-        <f t="array" ref="G14">_xlfn.LET(
+      <c r="G30" s="3" cm="1">
+        <f t="array" ref="G30">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,126,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13146,13 +13927,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" cm="1">
-        <f t="array" ref="D15">_xlfn.LET(
+      <c r="H30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="3" cm="1">
+        <f t="array" ref="D31">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,106,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13163,8 +13949,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E15" cm="1">
-        <f t="array" ref="E15">_xlfn.LET(
+      <c r="E31" s="3" cm="1">
+        <f t="array" ref="E31">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,106,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13174,8 +13960,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F15" cm="1">
-        <f t="array" ref="F15">_xlfn.LET(
+      <c r="F31" s="3" cm="1">
+        <f t="array" ref="F31">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,106,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13185,8 +13971,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G15" cm="1">
-        <f t="array" ref="G15">_xlfn.LET(
+      <c r="G31" s="3" cm="1">
+        <f t="array" ref="G31">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,106,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13196,16 +13982,454 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+      <c r="H31" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D32" s="10" cm="1">
+        <f t="array" ref="D32">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,112,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,112,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,112,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E32" s="10" cm="1">
+        <f t="array" ref="E32">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="10" cm="1">
+        <f t="array" ref="F32">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="10" cm="1">
+        <f t="array" ref="G32">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,107,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,112,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" ref="H32:H41" si="3">(2*E32*F32)/(E32+F32)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="10" cm="1">
+        <f t="array" ref="D33">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,109,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,109,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,109,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E33" s="10" cm="1">
+        <f t="array" ref="E33">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="10" cm="1">
+        <f t="array" ref="F33">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="10" cm="1">
+        <f t="array" ref="G33">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,104,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,109,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="10" cm="1">
+        <f t="array" ref="D34">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,110,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,110,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,110,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E34" s="10" cm="1">
+        <f t="array" ref="E34">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="10" cm="1">
+        <f t="array" ref="F34">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="10" cm="1">
+        <f t="array" ref="G34">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,105,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,110,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="10" cm="1">
+        <f t="array" ref="D35">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,131,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,131,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!E:E, _xlfn.SEQUENCE(4,1,131,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E35" s="10" cm="1">
+        <f t="array" ref="E35">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="10" cm="1">
+        <f t="array" ref="F35">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!H:H, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="10" cm="1">
+        <f t="array" ref="G35">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,126,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,131,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="10"/>
+      <c r="C36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D16" cm="1">
-        <f t="array" ref="D16">_xlfn.LET(
+      <c r="D36" s="10" cm="1">
+        <f t="array" ref="D36">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,111,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,111,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!E:E, _xlfn.SEQUENCE(1,1,111,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E36" s="10" cm="1">
+        <f t="array" ref="E36">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="10" cm="1">
+        <f t="array" ref="F36">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!H:H, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="10" cm="1">
+        <f t="array" ref="G36">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,106,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,111,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="18" cm="1">
+        <f t="array" ref="D37">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,122,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,122,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,122,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E37" s="18" cm="1">
+        <f t="array" ref="E37">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="18" cm="1">
+        <f t="array" ref="F37">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="18" cm="1">
+        <f t="array" ref="G37">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,117,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,122,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="18">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="18"/>
+      <c r="C38" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="18" cm="1">
+        <f t="array" ref="D38">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,119,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,119,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,119,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E38" s="18" cm="1">
+        <f t="array" ref="E38">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F38" s="18" cm="1">
+        <f t="array" ref="F38">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="18" cm="1">
+        <f t="array" ref="G38">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,114,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,119,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="18">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39" s="18"/>
+      <c r="C39" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="18" cm="1">
+        <f t="array" ref="D39">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,120,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,120,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,120,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E39" s="18" cm="1">
+        <f t="array" ref="E39">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F39" s="18" cm="1">
+        <f t="array" ref="F39">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="18" cm="1">
+        <f t="array" ref="G39">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,115,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,120,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="18">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="18" cm="1">
+        <f t="array" ref="D40">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,141,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,141,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!E:E, _xlfn.SEQUENCE(4,1,141,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E40" s="18" cm="1">
+        <f t="array" ref="E40">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="18" cm="1">
+        <f t="array" ref="F40">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!H:H, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="18" cm="1">
+        <f t="array" ref="G40">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,136,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,141,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="18">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="18"/>
+      <c r="C41" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="18" cm="1">
+        <f t="array" ref="D41">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,121,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,121,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!E:E, _xlfn.SEQUENCE(1,1,121,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E41" s="18" cm="1">
+        <f t="array" ref="E41">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F41" s="18" cm="1">
+        <f t="array" ref="F41">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!H:H, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="18" cm="1">
+        <f t="array" ref="G41">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,116,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,121,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="18">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="3" cm="1">
+        <f t="array" ref="D43">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,208,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13216,8 +14440,8 @@
 )</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="E16" cm="1">
-        <f t="array" ref="E16">_xlfn.LET(
+      <c r="E43" s="3" cm="1">
+        <f t="array" ref="E43">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,208,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13227,8 +14451,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F16" cm="1">
-        <f t="array" ref="F16">_xlfn.LET(
+      <c r="F43" s="3" cm="1">
+        <f t="array" ref="F43">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,208,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13238,8 +14462,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G16" cm="1">
-        <f t="array" ref="G16">_xlfn.LET(
+      <c r="G43" s="3" cm="1">
+        <f t="array" ref="G43">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,208,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13249,13 +14473,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" cm="1">
-        <f t="array" ref="D17">_xlfn.LET(
+      <c r="H43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="3" cm="1">
+        <f t="array" ref="D44">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,205,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13266,8 +14495,8 @@
 )</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="E17" cm="1">
-        <f t="array" ref="E17">_xlfn.LET(
+      <c r="E44" s="3" cm="1">
+        <f t="array" ref="E44">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,205,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13277,8 +14506,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F17" cm="1">
-        <f t="array" ref="F17">_xlfn.LET(
+      <c r="F44" s="3" cm="1">
+        <f t="array" ref="F44">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,205,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13288,8 +14517,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G17" cm="1">
-        <f t="array" ref="G17">_xlfn.LET(
+      <c r="G44" s="3" cm="1">
+        <f t="array" ref="G44">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,205,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13299,13 +14528,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" cm="1">
-        <f t="array" ref="D18">_xlfn.LET(
+      <c r="H44" s="3">
+        <f t="shared" si="2"/>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="3" cm="1">
+        <f t="array" ref="D45">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,206,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13316,8 +14550,8 @@
 )</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="E18" t="e" cm="1">
-        <f t="array" ref="E18">_xlfn.LET(
+      <c r="E45" s="3" t="e" cm="1">
+        <f t="array" ref="E45">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,206,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13327,8 +14561,8 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F18" cm="1">
-        <f t="array" ref="F18">_xlfn.LET(
+      <c r="F45" s="3" cm="1">
+        <f t="array" ref="F45">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,206,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13338,8 +14572,8 @@
 )</f>
         <v>0</v>
       </c>
-      <c r="G18" cm="1">
-        <f t="array" ref="G18">_xlfn.LET(
+      <c r="G45" s="3" cm="1">
+        <f t="array" ref="G45">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(20,1,206,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13349,13 +14583,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" cm="1">
-        <f t="array" ref="D19">_xlfn.LET(
+      <c r="H45" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="3" cm="1">
+        <f t="array" ref="D46">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,227,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13366,8 +14605,8 @@
 )</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="E19" t="e" cm="1">
-        <f t="array" ref="E19">_xlfn.LET(
+      <c r="E46" s="3" t="e" cm="1">
+        <f t="array" ref="E46">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,227,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13377,8 +14616,8 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" cm="1">
-        <f t="array" ref="F19">_xlfn.LET(
+      <c r="F46" s="3" cm="1">
+        <f t="array" ref="F46">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,227,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13388,8 +14627,8 @@
 )</f>
         <v>0</v>
       </c>
-      <c r="G19" cm="1">
-        <f t="array" ref="G19">_xlfn.LET(
+      <c r="G46" s="3" cm="1">
+        <f t="array" ref="G46">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(16,1,227,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13399,13 +14638,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" cm="1">
-        <f t="array" ref="D20">_xlfn.LET(
+      <c r="H46" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="3" cm="1">
+        <f t="array" ref="D47">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,207,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13416,8 +14660,8 @@
 )</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="E20" t="e" cm="1">
-        <f t="array" ref="E20">_xlfn.LET(
+      <c r="E47" s="3" t="e" cm="1">
+        <f t="array" ref="E47">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,207,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13427,8 +14671,8 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" cm="1">
-        <f t="array" ref="F20">_xlfn.LET(
+      <c r="F47" s="3" cm="1">
+        <f t="array" ref="F47">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,207,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13438,8 +14682,8 @@
 )</f>
         <v>0</v>
       </c>
-      <c r="G20" cm="1">
-        <f t="array" ref="G20">_xlfn.LET(
+      <c r="G47" s="3" cm="1">
+        <f t="array" ref="G47">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,207,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13449,19 +14693,240 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="H47" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="10" cm="1">
+        <f t="array" ref="D48">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,213,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,213,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,213,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E48" s="10" cm="1">
+        <f t="array" ref="E48">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F48" s="10" cm="1">
+        <f t="array" ref="F48">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
         <v>1</v>
       </c>
-      <c r="D22" cm="1">
-        <f t="array" ref="D22">_xlfn.LET(
+      <c r="G48" s="10" cm="1">
+        <f t="array" ref="G48">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,208,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,213,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H48" s="10">
+        <f>(2*E48*F48)/(E48+F48)</f>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="10" cm="1">
+        <f t="array" ref="D49">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,210,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,210,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,210,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E49" s="10" cm="1">
+        <f t="array" ref="E49">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F49" s="10" cm="1">
+        <f t="array" ref="F49">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="10" cm="1">
+        <f t="array" ref="G49">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,205,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,210,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H49" s="10">
+        <f t="shared" ref="H49:H52" si="4">(2*E49*F49)/(E49+F49)</f>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="10" cm="1">
+        <f t="array" ref="D50">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,211,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,211,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!E:E, _xlfn.SEQUENCE(5,1,211,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E50" s="10" t="e" cm="1">
+        <f t="array" ref="E50">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F50" s="10" cm="1">
+        <f t="array" ref="F50">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!F:F, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!H:H, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="10" cm="1">
+        <f t="array" ref="G50">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!I:I, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(5,1,206,20)),INDEX(results!G:G, _xlfn.SEQUENCE(5,1,211,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B51" s="10"/>
+      <c r="C51" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="10" cm="1">
+        <f t="array" ref="D51">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,232,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,232,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!E:E, _xlfn.SEQUENCE(4,1,232,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E51" s="10" t="e" cm="1">
+        <f t="array" ref="E51">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F51" s="10" cm="1">
+        <f t="array" ref="F51">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!F:F, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!H:H, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="10" cm="1">
+        <f t="array" ref="G51">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!I:I, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(4,1,227,20)),INDEX(results!G:G, _xlfn.SEQUENCE(4,1,232,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="10" cm="1">
+        <f t="array" ref="D52">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,212,20))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,212,20))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!E:E, _xlfn.SEQUENCE(1,1,212,20))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E52" s="10" t="e" cm="1">
+        <f t="array" ref="E52">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F52" s="10" cm="1">
+        <f t="array" ref="F52">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!F:F, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!H:H, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="10" cm="1">
+        <f t="array" ref="G52">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!I:I, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(1,1,207,20)),INDEX(results!G:G, _xlfn.SEQUENCE(1,1,212,20))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H52" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" cm="1">
+        <f t="array" ref="D54">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,2,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13472,8 +14937,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E22" cm="1">
-        <f t="array" ref="E22">_xlfn.LET(
+      <c r="E54" s="3" cm="1">
+        <f t="array" ref="E54">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,2,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13483,8 +14948,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F22" cm="1">
-        <f t="array" ref="F22">_xlfn.LET(
+      <c r="F54" s="3" cm="1">
+        <f t="array" ref="F54">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,2,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13494,8 +14959,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G22" cm="1">
-        <f t="array" ref="G22">_xlfn.LET(
+      <c r="G54" s="3" cm="1">
+        <f t="array" ref="G54">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,2,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13505,13 +14970,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
+      <c r="H54" s="3">
+        <f t="shared" ref="H54:H90" si="5">(2*E54*F54)/(E54+F54)</f>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D23" cm="1">
-        <f t="array" ref="D23">_xlfn.LET(
+      <c r="D55" s="3" cm="1">
+        <f t="array" ref="D55">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,22,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13522,8 +14992,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E23" cm="1">
-        <f t="array" ref="E23">_xlfn.LET(
+      <c r="E55" s="3" cm="1">
+        <f t="array" ref="E55">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,22,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13533,8 +15003,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F23" cm="1">
-        <f t="array" ref="F23">_xlfn.LET(
+      <c r="F55" s="3" cm="1">
+        <f t="array" ref="F55">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,22,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13544,8 +15014,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G23" cm="1">
-        <f t="array" ref="G23">_xlfn.LET(
+      <c r="G55" s="3" cm="1">
+        <f t="array" ref="G55">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,22,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13555,13 +15025,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
+      <c r="H55" s="3">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D24" cm="1">
-        <f t="array" ref="D24">_xlfn.LET(
+      <c r="D56" s="3" cm="1">
+        <f t="array" ref="D56">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,42,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13572,8 +15047,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E24" cm="1">
-        <f t="array" ref="E24">_xlfn.LET(
+      <c r="E56" s="3" cm="1">
+        <f t="array" ref="E56">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,42,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13583,8 +15058,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F24" cm="1">
-        <f t="array" ref="F24">_xlfn.LET(
+      <c r="F56" s="3" cm="1">
+        <f t="array" ref="F56">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,42,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13594,8 +15069,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G24" cm="1">
-        <f t="array" ref="G24">_xlfn.LET(
+      <c r="G56" s="3" cm="1">
+        <f t="array" ref="G56">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,42,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13605,13 +15080,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
+      <c r="H56" s="3">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D25" cm="1">
-        <f t="array" ref="D25">_xlfn.LET(
+      <c r="D57" s="3" cm="1">
+        <f t="array" ref="D57">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,62,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13622,8 +15102,8 @@
 )</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E25" cm="1">
-        <f t="array" ref="E25">_xlfn.LET(
+      <c r="E57" s="3" cm="1">
+        <f t="array" ref="E57">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,62,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13633,8 +15113,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F25" cm="1">
-        <f t="array" ref="F25">_xlfn.LET(
+      <c r="F57" s="3" cm="1">
+        <f t="array" ref="F57">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,62,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13644,8 +15124,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="G25" cm="1">
-        <f t="array" ref="G25">_xlfn.LET(
+      <c r="G57" s="3" cm="1">
+        <f t="array" ref="G57">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,62,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13655,13 +15135,18 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
+      <c r="H57" s="3">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D26" cm="1">
-        <f t="array" ref="D26">_xlfn.LET(
+      <c r="D58" s="3" cm="1">
+        <f t="array" ref="D58">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,82,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13672,8 +15157,8 @@
 )</f>
         <v>0.58823529411764708</v>
       </c>
-      <c r="E26" cm="1">
-        <f t="array" ref="E26">_xlfn.LET(
+      <c r="E58" s="3" cm="1">
+        <f t="array" ref="E58">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,82,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13683,8 +15168,8 @@
 )</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F26" cm="1">
-        <f t="array" ref="F26">_xlfn.LET(
+      <c r="F58" s="3" cm="1">
+        <f t="array" ref="F58">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,82,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13694,8 +15179,8 @@
 )</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="G26" cm="1">
-        <f t="array" ref="G26">_xlfn.LET(
+      <c r="G58" s="3" cm="1">
+        <f t="array" ref="G58">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,82,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13705,16 +15190,454 @@
 )</f>
         <v>0.98412698412698407</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="H58" s="3">
+        <f t="shared" si="5"/>
+        <v>0.24615384615384617</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B59" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D27" cm="1">
-        <f t="array" ref="D27">_xlfn.LET(
+      <c r="D59" s="10" cm="1">
+        <f t="array" ref="D59">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,2,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,2,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,2,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E59" s="10" cm="1">
+        <f t="array" ref="E59">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F59" s="10" cm="1">
+        <f t="array" ref="F59">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G59" s="10" cm="1">
+        <f t="array" ref="G59">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,2,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H59" s="10">
+        <f>(2*E59*F59)/(E59+F59)</f>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B60" s="10"/>
+      <c r="C60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="10" cm="1">
+        <f t="array" ref="D60">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,22,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,22,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,22,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E60" s="10" cm="1">
+        <f t="array" ref="E60">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F60" s="10" cm="1">
+        <f t="array" ref="F60">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G60" s="10" cm="1">
+        <f t="array" ref="G60">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,22,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H60" s="10">
+        <f t="shared" ref="H60:H63" si="6">(2*E60*F60)/(E60+F60)</f>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B61" s="10"/>
+      <c r="C61" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="10" cm="1">
+        <f t="array" ref="D61">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,42,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,42,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,42,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E61" s="10" cm="1">
+        <f t="array" ref="E61">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F61" s="10" cm="1">
+        <f t="array" ref="F61">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G61" s="10" cm="1">
+        <f t="array" ref="G61">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,42,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H61" s="10">
+        <f t="shared" si="6"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B62" s="10"/>
+      <c r="C62" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="10" cm="1">
+        <f t="array" ref="D62">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,62,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,62,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,62,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E62" s="10" cm="1">
+        <f t="array" ref="E62">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F62" s="10" cm="1">
+        <f t="array" ref="F62">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G62" s="10" cm="1">
+        <f t="array" ref="G62">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,62,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H62" s="10">
+        <f t="shared" si="6"/>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B63" s="10"/>
+      <c r="C63" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="10" cm="1">
+        <f t="array" ref="D63">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,82,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,82,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,82,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.60317460317460314</v>
+      </c>
+      <c r="E63" s="10" cm="1">
+        <f t="array" ref="E63">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F63" s="10" cm="1">
+        <f t="array" ref="F63">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G63" s="10" cm="1">
+        <f t="array" ref="G63">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,82,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="H63" s="10">
+        <f t="shared" si="6"/>
+        <v>0.24242424242424243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="18" cm="1">
+        <f t="array" ref="D64">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,12,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,12,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,12,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="18" cm="1">
+        <f t="array" ref="E64">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F64" s="18" cm="1">
+        <f t="array" ref="F64">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G64" s="18" cm="1">
+        <f t="array" ref="G64">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,12,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H64" s="18">
+        <f>(2*E64*F64)/(E64+F64)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="18"/>
+      <c r="C65" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="18" cm="1">
+        <f t="array" ref="D65">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,32,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,32,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,32,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E65" s="18" cm="1">
+        <f t="array" ref="E65">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F65" s="18" cm="1">
+        <f t="array" ref="F65">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G65" s="18" cm="1">
+        <f t="array" ref="G65">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,32,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H65" s="18">
+        <f t="shared" ref="H65:H68" si="7">(2*E65*F65)/(E65+F65)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="18"/>
+      <c r="C66" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="18" cm="1">
+        <f t="array" ref="D66">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,52,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,52,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,52,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E66" s="18" cm="1">
+        <f t="array" ref="E66">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F66" s="18" cm="1">
+        <f t="array" ref="F66">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G66" s="18" cm="1">
+        <f t="array" ref="G66">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,52,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H66" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="18"/>
+      <c r="C67" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="18" cm="1">
+        <f t="array" ref="D67">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,72,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,72,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,72,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="E67" s="18" cm="1">
+        <f t="array" ref="E67">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F67" s="18" cm="1">
+        <f t="array" ref="F67">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="G67" s="18" cm="1">
+        <f t="array" ref="G67">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,72,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H67" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="18"/>
+      <c r="C68" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="18" cm="1">
+        <f t="array" ref="D68">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,92,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,92,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,92,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E68" s="18" cm="1">
+        <f t="array" ref="E68">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F68" s="18" cm="1">
+        <f t="array" ref="F68">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G68" s="18" cm="1">
+        <f t="array" ref="G68">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,92,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H68" s="18">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" s="3" cm="1">
+        <f t="array" ref="D70">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,103,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13725,8 +15648,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E27" cm="1">
-        <f t="array" ref="E27">_xlfn.LET(
+      <c r="E70" s="3" cm="1">
+        <f t="array" ref="E70">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,103,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13736,8 +15659,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F27" cm="1">
-        <f t="array" ref="F27">_xlfn.LET(
+      <c r="F70" s="3" cm="1">
+        <f t="array" ref="F70">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,103,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13747,8 +15670,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G27" cm="1">
-        <f t="array" ref="G27">_xlfn.LET(
+      <c r="G70" s="3" cm="1">
+        <f t="array" ref="G70">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,103,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13758,13 +15681,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
+      <c r="H70" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D28" cm="1">
-        <f t="array" ref="D28">_xlfn.LET(
+      <c r="D71" s="3" cm="1">
+        <f t="array" ref="D71">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,123,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13775,8 +15703,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E28" cm="1">
-        <f t="array" ref="E28">_xlfn.LET(
+      <c r="E71" s="3" cm="1">
+        <f t="array" ref="E71">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,123,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13786,8 +15714,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F28" cm="1">
-        <f t="array" ref="F28">_xlfn.LET(
+      <c r="F71" s="3" cm="1">
+        <f t="array" ref="F71">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,123,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13797,8 +15725,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G28" cm="1">
-        <f t="array" ref="G28">_xlfn.LET(
+      <c r="G71" s="3" cm="1">
+        <f t="array" ref="G71">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,123,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13808,13 +15736,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
+      <c r="H71" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D29" cm="1">
-        <f t="array" ref="D29">_xlfn.LET(
+      <c r="D72" s="3" cm="1">
+        <f t="array" ref="D72">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,143,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13825,8 +15758,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E29" cm="1">
-        <f t="array" ref="E29">_xlfn.LET(
+      <c r="E72" s="3" cm="1">
+        <f t="array" ref="E72">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,143,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13836,8 +15769,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F29" cm="1">
-        <f t="array" ref="F29">_xlfn.LET(
+      <c r="F72" s="3" cm="1">
+        <f t="array" ref="F72">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,143,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13847,8 +15780,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G29" cm="1">
-        <f t="array" ref="G29">_xlfn.LET(
+      <c r="G72" s="3" cm="1">
+        <f t="array" ref="G72">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,143,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13858,13 +15791,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
+      <c r="H72" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D30" cm="1">
-        <f t="array" ref="D30">_xlfn.LET(
+      <c r="D73" s="3" cm="1">
+        <f t="array" ref="D73">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,163,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13875,8 +15813,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E30" cm="1">
-        <f t="array" ref="E30">_xlfn.LET(
+      <c r="E73" s="3" cm="1">
+        <f t="array" ref="E73">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,163,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13886,8 +15824,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F30" cm="1">
-        <f t="array" ref="F30">_xlfn.LET(
+      <c r="F73" s="3" cm="1">
+        <f t="array" ref="F73">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,163,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13897,8 +15835,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G30" cm="1">
-        <f t="array" ref="G30">_xlfn.LET(
+      <c r="G73" s="3" cm="1">
+        <f t="array" ref="G73">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,163,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13908,13 +15846,18 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C31" t="s">
+      <c r="H73" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D31" cm="1">
-        <f t="array" ref="D31">_xlfn.LET(
+      <c r="D74" s="3" cm="1">
+        <f t="array" ref="D74">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,183,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13925,8 +15868,8 @@
 )</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="E31" cm="1">
-        <f t="array" ref="E31">_xlfn.LET(
+      <c r="E74" s="3" cm="1">
+        <f t="array" ref="E74">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,183,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13936,8 +15879,8 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="F31" cm="1">
-        <f t="array" ref="F31">_xlfn.LET(
+      <c r="F74" s="3" cm="1">
+        <f t="array" ref="F74">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,183,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -13947,8 +15890,8 @@
 )</f>
         <v>0.5</v>
       </c>
-      <c r="G31" cm="1">
-        <f t="array" ref="G31">_xlfn.LET(
+      <c r="G74" s="3" cm="1">
+        <f t="array" ref="G74">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,183,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13958,16 +15901,454 @@
 )</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="H74" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B75" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D32" cm="1">
-        <f t="array" ref="D32">_xlfn.LET(
+      <c r="D75" s="10" cm="1">
+        <f t="array" ref="D75">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,103,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,103,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,103,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E75" s="10" cm="1">
+        <f t="array" ref="E75">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F75" s="10" cm="1">
+        <f t="array" ref="F75">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G75" s="10" cm="1">
+        <f t="array" ref="G75">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,103,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H75" s="10">
+        <f>(2*E75*F75)/(E75+F75)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B76" s="10"/>
+      <c r="C76" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="10" cm="1">
+        <f t="array" ref="D76">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,123,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,123,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,123,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E76" s="10" cm="1">
+        <f t="array" ref="E76">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F76" s="10" cm="1">
+        <f t="array" ref="F76">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G76" s="10" cm="1">
+        <f t="array" ref="G76">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,123,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H76" s="10">
+        <f t="shared" ref="H76:H79" si="8">(2*E76*F76)/(E76+F76)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B77" s="10"/>
+      <c r="C77" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="10" cm="1">
+        <f t="array" ref="D77">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,143,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,143,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,143,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E77" s="10" cm="1">
+        <f t="array" ref="E77">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F77" s="10" cm="1">
+        <f t="array" ref="F77">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G77" s="10" cm="1">
+        <f t="array" ref="G77">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,143,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H77" s="10">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B78" s="10"/>
+      <c r="C78" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="10" cm="1">
+        <f t="array" ref="D78">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,163,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,163,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,163,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E78" s="10" cm="1">
+        <f t="array" ref="E78">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F78" s="10" cm="1">
+        <f t="array" ref="F78">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G78" s="10" cm="1">
+        <f t="array" ref="G78">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,163,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H78" s="10">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D79" s="10" cm="1">
+        <f t="array" ref="D79">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,183,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,183,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,183,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E79" s="10" cm="1">
+        <f t="array" ref="E79">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F79" s="10" cm="1">
+        <f t="array" ref="F79">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G79" s="10" cm="1">
+        <f t="array" ref="G79">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,183,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H79" s="10">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B80" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" s="18" cm="1">
+        <f t="array" ref="D80">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,113,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,113,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,113,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E80" s="18" cm="1">
+        <f t="array" ref="E80">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F80" s="18" cm="1">
+        <f t="array" ref="F80">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G80" s="18" cm="1">
+        <f t="array" ref="G80">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,113,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H80" s="18">
+        <f>(2*E80*F80)/(E80+F80)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B81" s="18"/>
+      <c r="C81" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="18" cm="1">
+        <f t="array" ref="D81">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,133,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,133,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,133,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E81" s="18" cm="1">
+        <f t="array" ref="E81">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F81" s="18" cm="1">
+        <f t="array" ref="F81">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G81" s="18" cm="1">
+        <f t="array" ref="G81">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,133,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H81" s="18">
+        <f t="shared" ref="H81:H84" si="9">(2*E81*F81)/(E81+F81)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B82" s="18"/>
+      <c r="C82" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="18" cm="1">
+        <f t="array" ref="D82">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,153,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,153,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,153,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E82" s="18" cm="1">
+        <f t="array" ref="E82">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F82" s="18" cm="1">
+        <f t="array" ref="F82">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G82" s="18" cm="1">
+        <f t="array" ref="G82">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,153,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H82" s="18">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B83" s="18"/>
+      <c r="C83" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D83" s="18" cm="1">
+        <f t="array" ref="D83">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,173,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,173,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,173,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E83" s="18" cm="1">
+        <f t="array" ref="E83">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F83" s="18" cm="1">
+        <f t="array" ref="F83">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G83" s="18" cm="1">
+        <f t="array" ref="G83">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,173,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H83" s="18">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B84" s="18"/>
+      <c r="C84" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" s="18" cm="1">
+        <f t="array" ref="D84">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,193,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,193,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,193,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E84" s="18" cm="1">
+        <f t="array" ref="E84">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="F84" s="18" cm="1">
+        <f t="array" ref="F84">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G84" s="18" cm="1">
+        <f t="array" ref="G84">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,193,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H84" s="18">
+        <f t="shared" si="9"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B86" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3" cm="1">
+        <f t="array" ref="D86">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,204,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -13978,8 +16359,8 @@
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E32" cm="1">
-        <f t="array" ref="E32">_xlfn.LET(
+      <c r="E86" s="3" cm="1">
+        <f t="array" ref="E86">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,204,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -13989,8 +16370,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F32" cm="1">
-        <f t="array" ref="F32">_xlfn.LET(
+      <c r="F86" s="3" cm="1">
+        <f t="array" ref="F86">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,204,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -14000,8 +16381,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G32" cm="1">
-        <f t="array" ref="G32">_xlfn.LET(
+      <c r="G86" s="3" cm="1">
+        <f t="array" ref="G86">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,204,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14011,13 +16392,18 @@
 )</f>
         <v>0.95238095238095233</v>
       </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
+      <c r="H86" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D33" cm="1">
-        <f t="array" ref="D33">_xlfn.LET(
+      <c r="D87" s="3" cm="1">
+        <f t="array" ref="D87">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,224,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -14028,8 +16414,8 @@
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E33" cm="1">
-        <f t="array" ref="E33">_xlfn.LET(
+      <c r="E87" s="3" cm="1">
+        <f t="array" ref="E87">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,224,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14039,8 +16425,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F33" cm="1">
-        <f t="array" ref="F33">_xlfn.LET(
+      <c r="F87" s="3" cm="1">
+        <f t="array" ref="F87">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,224,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -14050,8 +16436,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G33" cm="1">
-        <f t="array" ref="G33">_xlfn.LET(
+      <c r="G87" s="3" cm="1">
+        <f t="array" ref="G87">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,224,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14061,13 +16447,18 @@
 )</f>
         <v>0.95238095238095233</v>
       </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
+      <c r="H87" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D34" cm="1">
-        <f t="array" ref="D34">_xlfn.LET(
+      <c r="D88" s="3" cm="1">
+        <f t="array" ref="D88">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,244,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -14078,8 +16469,8 @@
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E34" cm="1">
-        <f t="array" ref="E34">_xlfn.LET(
+      <c r="E88" s="3" cm="1">
+        <f t="array" ref="E88">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,244,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14089,8 +16480,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F34" cm="1">
-        <f t="array" ref="F34">_xlfn.LET(
+      <c r="F88" s="3" cm="1">
+        <f t="array" ref="F88">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,244,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -14100,8 +16491,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G34" cm="1">
-        <f t="array" ref="G34">_xlfn.LET(
+      <c r="G88" s="3" cm="1">
+        <f t="array" ref="G88">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,244,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14111,13 +16502,18 @@
 )</f>
         <v>0.95238095238095233</v>
       </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
+      <c r="H88" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D35" cm="1">
-        <f t="array" ref="D35">_xlfn.LET(
+      <c r="D89" s="3" cm="1">
+        <f t="array" ref="D89">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,264,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -14128,8 +16524,8 @@
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E35" cm="1">
-        <f t="array" ref="E35">_xlfn.LET(
+      <c r="E89" s="3" cm="1">
+        <f t="array" ref="E89">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,264,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14139,8 +16535,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F35" cm="1">
-        <f t="array" ref="F35">_xlfn.LET(
+      <c r="F89" s="3" cm="1">
+        <f t="array" ref="F89">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,264,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -14150,8 +16546,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G35" cm="1">
-        <f t="array" ref="G35">_xlfn.LET(
+      <c r="G89" s="3" cm="1">
+        <f t="array" ref="G89">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,264,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14161,13 +16557,18 @@
 )</f>
         <v>0.95238095238095233</v>
       </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C36" t="s">
+      <c r="H89" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D36" cm="1">
-        <f t="array" ref="D36">_xlfn.LET(
+      <c r="D90" s="3" cm="1">
+        <f t="array" ref="D90">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,284,5),
   _xlpm.fValues, INDEX(results!F:F, _xlpm.rows),
   _xlpm.iValues, INDEX(results!I:I, _xlpm.rows),
@@ -14178,8 +16579,8 @@
 )</f>
         <v>0.60504201680672265</v>
       </c>
-      <c r="E36" cm="1">
-        <f t="array" ref="E36">_xlfn.LET(
+      <c r="E90" s="3" cm="1">
+        <f t="array" ref="E90">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,284,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14189,8 +16590,8 @@
 )</f>
         <v>0.8</v>
       </c>
-      <c r="F36" cm="1">
-        <f t="array" ref="F36">_xlfn.LET(
+      <c r="F90" s="3" cm="1">
+        <f t="array" ref="F90">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,284,5),
   _xlpm.rF, INDEX(results!F:F, _xlpm.rows),
   _xlpm.rH, INDEX(results!H:H, _xlpm.rows),
@@ -14200,8 +16601,8 @@
 )</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G36" cm="1">
-        <f t="array" ref="G36">_xlfn.LET(
+      <c r="G90" s="3" cm="1">
+        <f t="array" ref="G90">_xlfn.LET(
   _xlpm.rows, _xlfn.SEQUENCE(4,1,284,5),
   _xlpm.rI, INDEX(results!I:I, _xlpm.rows),
   _xlpm.rG, INDEX(results!G:G, _xlpm.rows),
@@ -14210,6 +16611,227 @@
   _xlpm.num/_xlpm.denom
 )</f>
         <v>0.95238095238095233</v>
+      </c>
+      <c r="H90" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3380281690140845</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B91" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" s="10" cm="1">
+        <f t="array" ref="D91">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,204,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,204,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,204,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E91" s="10" cm="1">
+        <f t="array" ref="E91">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F91" s="10" cm="1">
+        <f t="array" ref="F91">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G91" s="10" cm="1">
+        <f t="array" ref="G91">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,204,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H91" s="10">
+        <f>(2*E91*F91)/(E91+F91)</f>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B92" s="10"/>
+      <c r="C92" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="10" cm="1">
+        <f t="array" ref="D92">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,224,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,224,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,224,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E92" s="10" cm="1">
+        <f t="array" ref="E92">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F92" s="10" cm="1">
+        <f t="array" ref="F92">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G92" s="10" cm="1">
+        <f t="array" ref="G92">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,224,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H92" s="10">
+        <f t="shared" ref="H92:H95" si="10">(2*E92*F92)/(E92+F92)</f>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B93" s="10"/>
+      <c r="C93" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D93" s="10" cm="1">
+        <f t="array" ref="D93">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,244,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,244,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,244,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E93" s="10" cm="1">
+        <f t="array" ref="E93">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F93" s="10" cm="1">
+        <f t="array" ref="F93">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G93" s="10" cm="1">
+        <f t="array" ref="G93">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,244,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H93" s="10">
+        <f t="shared" si="10"/>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B94" s="10"/>
+      <c r="C94" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D94" s="10" cm="1">
+        <f t="array" ref="D94">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,264,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,264,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,264,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E94" s="10" cm="1">
+        <f t="array" ref="E94">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F94" s="10" cm="1">
+        <f t="array" ref="F94">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G94" s="10" cm="1">
+        <f t="array" ref="G94">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,264,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H94" s="10">
+        <f t="shared" si="10"/>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B95" s="10"/>
+      <c r="C95" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" s="10" cm="1">
+        <f t="array" ref="D95">_xlfn.LET(
+  _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,284,5))),
+  _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,284,5))),
+  _xlpm.valuesE, SUM(INDEX(results!E:E, _xlfn.SEQUENCE(2,1,284,5))),
+  SUM(_xlpm.valuesF + _xlpm.valuesI)/(_xlpm.valuesE)
+)</f>
+        <v>0.69841269841269837</v>
+      </c>
+      <c r="E95" s="10" cm="1">
+        <f t="array" ref="E95">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesG)
+)</f>
+        <v>0.8</v>
+      </c>
+      <c r="F95" s="10" cm="1">
+        <f t="array" ref="F95">_xlfn.LET(
+ _xlpm.valuesF, SUM(INDEX(results!F:F, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesH, SUM(INDEX(results!H:H, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesF / (_xlpm.valuesF + _xlpm.valuesH)
+)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G95" s="10" cm="1">
+        <f t="array" ref="G95">_xlfn.LET(
+ _xlpm.valuesI, SUM(INDEX(results!I:I, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesG, SUM(INDEX(results!G:G, _xlfn.SEQUENCE(2,1,284,5))),
+ _xlpm.valuesI / (_xlpm.valuesI + _xlpm.valuesG)
+)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="H95" s="10">
+        <f t="shared" si="10"/>
+        <v>0.55813953488372092</v>
       </c>
     </row>
   </sheetData>
@@ -14221,8 +16843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13FB626-F218-4B99-B9CF-F14B8A51FAA4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="76" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>